<commit_message>
Adicionado algumas tratativas no main workflow
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Paramater</t>
   </si>
@@ -57,10 +57,7 @@
     <t xml:space="preserve">element_timeout</t>
   </si>
   <si>
-    <t xml:space="preserve">parametro2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valor2</t>
+    <t xml:space="preserve">max_retry</t>
   </si>
 </sst>
 </file>
@@ -377,7 +374,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -435,8 +432,8 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
+      <c r="B3" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="C3" s="3"/>
     </row>

</xml_diff>